<commit_message>
wrote indv correlation fn
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/annot_results.xlsx
+++ b/Outputs/Annotation/annot_results.xlsx
@@ -8174,7 +8174,7 @@
         <v>0.0000000178519669484774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000406667807086315</v>
+        <v>0.0000406667807086316</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -8379,10 +8379,10 @@
         <v>1.50535400752026</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000475639853287725</v>
+        <v>0.0000475639853287726</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
@@ -8483,10 +8483,10 @@
         <v>1.80212684967551</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000499847719483916</v>
+        <v>0.0000499847719483915</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -8587,10 +8587,10 @@
         <v>2.09431049210052</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0000517922239009611</v>
+        <v>0.0000517922239009609</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F6" t="s">
         <v>90</v>
@@ -8794,7 +8794,7 @@
         <v>0.000110008275103165</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
@@ -8894,7 +8894,7 @@
         <v>0.000111361244672891</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F9" t="s">
         <v>122</v>
@@ -8998,7 +8998,7 @@
         <v>0.000112205604722291</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F10" t="s">
         <v>133</v>
@@ -9097,10 +9097,10 @@
         <v>1.04982890375572</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000126131019936542</v>
+        <v>0.000126131019936541</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0287326463415442</v>
+        <v>0.0287326463415441</v>
       </c>
       <c r="F11" t="s">
         <v>143</v>
@@ -9303,7 +9303,7 @@
         <v>0.986049090397621</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000192246012402054</v>
+        <v>0.000192246012402053</v>
       </c>
       <c r="E13" t="n">
         <v>0.032545879390594</v>
@@ -9717,7 +9717,7 @@
         <v>1.33076563688241</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000254639461413522</v>
+        <v>0.000254639461413521</v>
       </c>
       <c r="E17" t="n">
         <v>0.0362542933187501</v>
@@ -9928,7 +9928,7 @@
         <v>0.000380908914516266</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0482061392926697</v>
+        <v>0.0482061392926696</v>
       </c>
       <c r="F19" t="s">
         <v>219</v>
@@ -10131,7 +10131,7 @@
         <v>2.11985942237007</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000440559084185693</v>
+        <v>0.000440559084185694</v>
       </c>
       <c r="E21" t="n">
         <v>0.0501796796887505</v>
@@ -10233,7 +10233,7 @@
         <v>1.91995019137173</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000500571753448369</v>
+        <v>0.000500571753448367</v>
       </c>
       <c r="E22" t="n">
         <v>0.0521990821189653</v>
@@ -10335,7 +10335,7 @@
         <v>1.61125465202653</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000504117562167356</v>
+        <v>0.000504117562167355</v>
       </c>
       <c r="E23" t="n">
         <v>0.0521990821189653</v>
@@ -10439,7 +10439,7 @@
         <v>2.19572074738617</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000536816012583926</v>
+        <v>0.000536816012583925</v>
       </c>
       <c r="E24" t="n">
         <v>0.0531681250724427</v>
@@ -10849,7 +10849,7 @@
         <v>2.5917608012007</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000922568990829643</v>
+        <v>0.000922568990829641</v>
       </c>
       <c r="E28" t="n">
         <v>0.0764489881865432</v>
@@ -11060,7 +11060,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F30" t="s">
         <v>328</v>
@@ -11162,7 +11162,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F31" t="s">
         <v>328</v>
@@ -11264,7 +11264,7 @@
         <v>0.00105194943882193</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F32" t="s">
         <v>342</v>
@@ -11366,7 +11366,7 @@
         <v>0.00105453471953679</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F33" t="s">
         <v>350</v>
@@ -11468,7 +11468,7 @@
         <v>0.00108883939495889</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0775117544286357</v>
+        <v>0.0775117544286356</v>
       </c>
       <c r="F34" t="s">
         <v>361</v>
@@ -11572,7 +11572,7 @@
         <v>0.0013671855217853</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0943772308674821</v>
+        <v>0.094377230867482</v>
       </c>
       <c r="F35" t="s">
         <v>371</v>
@@ -11673,7 +11673,7 @@
         <v>2.28004007337048</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00175062336032303</v>
+        <v>0.00175062336032302</v>
       </c>
       <c r="E36" t="n">
         <v>0.115407122551921</v>
@@ -11773,7 +11773,7 @@
         <v>2.22193178182585</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00177315596545972</v>
+        <v>0.00177315596545971</v>
       </c>
       <c r="E37" t="n">
         <v>0.115407122551921</v>
@@ -12805,7 +12805,7 @@
         <v>1.10076053003269</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00256069584580062</v>
+        <v>0.00256069584580061</v>
       </c>
       <c r="E47" t="n">
         <v>0.127772460423391</v>
@@ -12957,7 +12957,7 @@
         <v>35</v>
       </c>
       <c r="T48" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U48" t="n">
         <v>611583.803921569</v>
@@ -13115,7 +13115,7 @@
         <v>1.74722767046515</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0028370075723866</v>
+        <v>0.00283700757238659</v>
       </c>
       <c r="E50" t="n">
         <v>0.134536691710072</v>
@@ -13525,7 +13525,7 @@
         <v>1.87754894817857</v>
       </c>
       <c r="D54" t="n">
-        <v>0.00308619616311079</v>
+        <v>0.0030861961631108</v>
       </c>
       <c r="E54" t="n">
         <v>0.135199131914738</v>
@@ -14033,7 +14033,7 @@
         <v>1.5984185900808</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00369826788451145</v>
+        <v>0.00369826788451144</v>
       </c>
       <c r="E59" t="n">
         <v>0.146018369479691</v>
@@ -14354,7 +14354,7 @@
         <v>609</v>
       </c>
       <c r="G62" t="n">
-        <v>15.9894380767719</v>
+        <v>15.989438076772</v>
       </c>
       <c r="H62" t="n">
         <v>15.4535504246111</v>
@@ -14600,10 +14600,10 @@
         <v>100</v>
       </c>
       <c r="U64" t="n">
-        <v>639738.190476191</v>
+        <v>639738.19047619</v>
       </c>
       <c r="V64" t="n">
-        <v>639738.190476191</v>
+        <v>639738.19047619</v>
       </c>
       <c r="W64" t="s">
         <v>43</v>
@@ -14757,7 +14757,7 @@
         <v>-1.03719098907359</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00463820694388655</v>
+        <v>0.00463820694388654</v>
       </c>
       <c r="E66" t="n">
         <v>0.161109582380577</v>
@@ -15117,7 +15117,7 @@
         <v>35</v>
       </c>
       <c r="T69" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U69" t="n">
         <v>138049.460784314</v>
@@ -15171,7 +15171,7 @@
         <v>-1.09646153941116</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00480924126509185</v>
+        <v>0.00480924126509184</v>
       </c>
       <c r="E70" t="n">
         <v>0.161109582380577</v>
@@ -15273,7 +15273,7 @@
         <v>1.65173907709379</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00516491822274916</v>
+        <v>0.00516491822274915</v>
       </c>
       <c r="E71" t="n">
         <v>0.170517155238008</v>
@@ -15479,7 +15479,7 @@
         <v>1.54031082907751</v>
       </c>
       <c r="D73" t="n">
-        <v>0.00541259787370311</v>
+        <v>0.0054125978737031</v>
       </c>
       <c r="E73" t="n">
         <v>0.173660534595714</v>
@@ -15683,10 +15683,10 @@
         <v>-1.43617464044618</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00610288959285422</v>
+        <v>0.00610288959285423</v>
       </c>
       <c r="E75" t="n">
-        <v>0.190443595787971</v>
+        <v>0.190443595787972</v>
       </c>
       <c r="F75" t="s">
         <v>730</v>
@@ -15785,7 +15785,7 @@
         <v>1.72026699754165</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00642796743910863</v>
+        <v>0.00642796743910865</v>
       </c>
       <c r="E76" t="n">
         <v>0.197877159814723</v>
@@ -15889,7 +15889,7 @@
         <v>0.697530163216005</v>
       </c>
       <c r="D77" t="n">
-        <v>0.00670714671808456</v>
+        <v>0.00670714671808457</v>
       </c>
       <c r="E77" t="n">
         <v>0.198403812483892</v>
@@ -15991,7 +15991,7 @@
         <v>0.963481828171481</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00698817479448877</v>
+        <v>0.00698817479448876</v>
       </c>
       <c r="E78" t="n">
         <v>0.198403812483892</v>
@@ -16095,7 +16095,7 @@
         <v>3.03596056752893</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0070305610038565</v>
+        <v>0.00703056100385651</v>
       </c>
       <c r="E79" t="n">
         <v>0.198403812483892</v>
@@ -16303,7 +16303,7 @@
         <v>1.26212292928929</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00711076042683458</v>
+        <v>0.00711076042683457</v>
       </c>
       <c r="E81" t="n">
         <v>0.198403812483892</v>
@@ -16555,7 +16555,7 @@
         <v>35</v>
       </c>
       <c r="T83" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U83" t="n">
         <v>104827.980392157</v>
@@ -16713,7 +16713,7 @@
         <v>1.26366052895703</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00722893610015938</v>
+        <v>0.00722893610015937</v>
       </c>
       <c r="E85" t="n">
         <v>0.198403812483892</v>
@@ -16815,7 +16815,7 @@
         <v>1.99233523129815</v>
       </c>
       <c r="D86" t="n">
-        <v>0.0073947544966017</v>
+        <v>0.00739475449660171</v>
       </c>
       <c r="E86" t="n">
         <v>0.200538699324508</v>
@@ -17537,7 +17537,7 @@
         <v>2.51435325201981</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00884745745358602</v>
+        <v>0.00884745745358603</v>
       </c>
       <c r="E93" t="n">
         <v>0.219946192103018</v>
@@ -17847,10 +17847,10 @@
         <v>1.33902553078093</v>
       </c>
       <c r="D96" t="n">
-        <v>0.00912105820259549</v>
+        <v>0.0091210582025955</v>
       </c>
       <c r="E96" t="n">
-        <v>0.221040112611835</v>
+        <v>0.221040112611836</v>
       </c>
       <c r="F96" t="s">
         <v>904</v>
@@ -18051,7 +18051,7 @@
         <v>1.76072590332704</v>
       </c>
       <c r="D98" t="n">
-        <v>0.00938134437347441</v>
+        <v>0.00938134437347442</v>
       </c>
       <c r="E98" t="n">
         <v>0.22261148419557</v>
@@ -18257,7 +18257,7 @@
         <v>1.82034483729149</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00972177970932419</v>
+        <v>0.00972177970932418</v>
       </c>
       <c r="E100" t="n">
         <v>0.225981777324903</v>
@@ -18359,7 +18359,7 @@
         <v>1.63103264825839</v>
       </c>
       <c r="D101" t="n">
-        <v>0.00984353580157741</v>
+        <v>0.0098435358015774</v>
       </c>
       <c r="E101" t="n">
         <v>0.226500753090842</v>
@@ -19281,10 +19281,10 @@
         <v>0.626816037819076</v>
       </c>
       <c r="D110" t="n">
-        <v>0.011550325673299</v>
+        <v>0.0115503256732989</v>
       </c>
       <c r="E110" t="n">
-        <v>0.243626313738658</v>
+        <v>0.243626313738657</v>
       </c>
       <c r="F110" t="s">
         <v>1021</v>
@@ -20302,7 +20302,7 @@
         <v>0.0128191613675105</v>
       </c>
       <c r="E120" t="n">
-        <v>0.247474996569398</v>
+        <v>0.247474996569399</v>
       </c>
       <c r="F120" t="s">
         <v>1101</v>
@@ -20404,7 +20404,7 @@
         <v>0.0130184057604316</v>
       </c>
       <c r="E121" t="n">
-        <v>0.249209481699691</v>
+        <v>0.24920948169969</v>
       </c>
       <c r="F121" t="s">
         <v>1109</v>
@@ -20607,7 +20607,7 @@
         <v>2.41635984686688</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0135023421528918</v>
+        <v>0.0135023421528919</v>
       </c>
       <c r="E123" t="n">
         <v>0.254201119208989</v>
@@ -24027,7 +24027,7 @@
         <v>35</v>
       </c>
       <c r="T156" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U156" t="n">
         <v>320818.843137255</v>
@@ -24287,7 +24287,7 @@
         <v>2.09123850802625</v>
       </c>
       <c r="D159" t="n">
-        <v>0.0199907411699751</v>
+        <v>0.019990741169975</v>
       </c>
       <c r="E159" t="n">
         <v>0.290056741307027</v>
@@ -25011,7 +25011,7 @@
         <v>1.21762092344371</v>
       </c>
       <c r="D166" t="n">
-        <v>0.0210472208862265</v>
+        <v>0.0210472208862264</v>
       </c>
       <c r="E166" t="n">
         <v>0.292351031578194</v>
@@ -25523,7 +25523,7 @@
         <v>0.867853197341834</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0226620463765855</v>
+        <v>0.0226620463765856</v>
       </c>
       <c r="E171" t="n">
         <v>0.302772694851184</v>
@@ -25729,7 +25729,7 @@
         <v>0.78371578317638</v>
       </c>
       <c r="D173" t="n">
-        <v>0.0228158223606759</v>
+        <v>0.022815822360676</v>
       </c>
       <c r="E173" t="n">
         <v>0.302772694851184</v>
@@ -25983,7 +25983,7 @@
         <v>35</v>
       </c>
       <c r="T175" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U175" t="n">
         <v>14629.5392156863</v>
@@ -26761,7 +26761,7 @@
         <v>1.57761266392044</v>
       </c>
       <c r="D183" t="n">
-        <v>0.0245691002586501</v>
+        <v>0.02456910025865</v>
       </c>
       <c r="E183" t="n">
         <v>0.31093561327336</v>
@@ -26865,10 +26865,10 @@
         <v>0.27905489843125</v>
       </c>
       <c r="D184" t="n">
-        <v>0.0248594505744229</v>
+        <v>0.024859450574423</v>
       </c>
       <c r="E184" t="n">
-        <v>0.312871980157654</v>
+        <v>0.312871980157655</v>
       </c>
       <c r="F184" t="s">
         <v>1610</v>
@@ -27901,7 +27901,7 @@
         <v>1.25376454302494</v>
       </c>
       <c r="D194" t="n">
-        <v>0.0268198605739047</v>
+        <v>0.0268198605739048</v>
       </c>
       <c r="E194" t="n">
         <v>0.320208023246158</v>
@@ -28211,7 +28211,7 @@
         <v>0.934103101296284</v>
       </c>
       <c r="D197" t="n">
-        <v>0.027011298152027</v>
+        <v>0.0270112981520271</v>
       </c>
       <c r="E197" t="n">
         <v>0.320477797866238</v>
@@ -28420,7 +28420,7 @@
         <v>0.0276051011071821</v>
       </c>
       <c r="E199" t="n">
-        <v>0.324146496505983</v>
+        <v>0.324146496505984</v>
       </c>
       <c r="F199" t="s">
         <v>1725</v>
@@ -30573,7 +30573,7 @@
         <v>1.22119471051002</v>
       </c>
       <c r="D220" t="n">
-        <v>0.0313979597922136</v>
+        <v>0.0313979597922135</v>
       </c>
       <c r="E220" t="n">
         <v>0.334574251532132</v>
@@ -30782,7 +30782,7 @@
         <v>0.0318779053495754</v>
       </c>
       <c r="E222" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F222" t="s">
         <v>1908</v>
@@ -30881,10 +30881,10 @@
         <v>2.26264357683325</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0319603715053673</v>
+        <v>0.0319603715053674</v>
       </c>
       <c r="E223" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F223" t="s">
         <v>1918</v>
@@ -30986,7 +30986,7 @@
         <v>0.0320126471951682</v>
       </c>
       <c r="E224" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F224" t="s">
         <v>1925</v>
@@ -31397,7 +31397,7 @@
         <v>1.78887655907102</v>
       </c>
       <c r="D228" t="n">
-        <v>0.0337919159899819</v>
+        <v>0.0337919159899818</v>
       </c>
       <c r="E228" t="n">
         <v>0.344552495084485</v>
@@ -31415,7 +31415,7 @@
         <v>14.6473805435874</v>
       </c>
       <c r="J228" t="n">
-        <v>3.4554570786045</v>
+        <v>3.45545707860451</v>
       </c>
       <c r="K228" t="s">
         <v>1961</v>
@@ -31499,7 +31499,7 @@
         <v>0.99704828479797</v>
       </c>
       <c r="D229" t="n">
-        <v>0.0338290806249597</v>
+        <v>0.0338290806249596</v>
       </c>
       <c r="E229" t="n">
         <v>0.344552495084485</v>
@@ -32115,7 +32115,7 @@
         <v>0.345489069906911</v>
       </c>
       <c r="D235" t="n">
-        <v>0.0346714061628505</v>
+        <v>0.0346714061628504</v>
       </c>
       <c r="E235" t="n">
         <v>0.344552495084485</v>
@@ -32336,7 +32336,7 @@
         <v>16.7343818564733</v>
       </c>
       <c r="I237" t="n">
-        <v>16.3377273626701</v>
+        <v>16.33772736267</v>
       </c>
       <c r="J237" t="n">
         <v>1.36152590482721</v>
@@ -32425,7 +32425,7 @@
         <v>1.74087635676352</v>
       </c>
       <c r="D238" t="n">
-        <v>0.0350155554167378</v>
+        <v>0.0350155554167379</v>
       </c>
       <c r="E238" t="n">
         <v>0.344552495084485</v>
@@ -33449,7 +33449,7 @@
         <v>1.80708411033922</v>
       </c>
       <c r="D248" t="n">
-        <v>0.0378469627388461</v>
+        <v>0.037846962738846</v>
       </c>
       <c r="E248" t="n">
         <v>0.355763774130317</v>
@@ -34189,7 +34189,7 @@
         <v>27.2048783401882</v>
       </c>
       <c r="J255" t="n">
-        <v>2.16064520185301</v>
+        <v>2.160645201853</v>
       </c>
       <c r="K255" t="s">
         <v>2161</v>
@@ -34375,7 +34375,7 @@
         <v>1.27522696767494</v>
       </c>
       <c r="D257" t="n">
-        <v>0.0394247070068917</v>
+        <v>0.0394247070068918</v>
       </c>
       <c r="E257" t="n">
         <v>0.357433512293212</v>
@@ -35043,7 +35043,7 @@
         <v>35</v>
       </c>
       <c r="T263" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U263" t="n">
         <v>515977.68627451</v>
@@ -35145,7 +35145,7 @@
         <v>35</v>
       </c>
       <c r="T264" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U264" t="n">
         <v>515977.68627451</v>
@@ -35199,7 +35199,7 @@
         <v>0.961685940676187</v>
       </c>
       <c r="D265" t="n">
-        <v>0.0404195812337836</v>
+        <v>0.0404195812337835</v>
       </c>
       <c r="E265" t="n">
         <v>0.357456311668854</v>
@@ -35211,7 +35211,7 @@
         <v>28.0202647722528</v>
       </c>
       <c r="H265" t="n">
-        <v>28.9819507129289</v>
+        <v>28.981950712929</v>
       </c>
       <c r="I265" t="n">
         <v>28.1251759657811</v>
@@ -35410,7 +35410,7 @@
         <v>0.0408089847599079</v>
       </c>
       <c r="E267" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F267" t="s">
         <v>2252</v>
@@ -35512,7 +35512,7 @@
         <v>0.0410740982767807</v>
       </c>
       <c r="E268" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F268" t="s">
         <v>2259</v>
@@ -35614,7 +35614,7 @@
         <v>0.0411672875092047</v>
       </c>
       <c r="E269" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F269" t="s">
         <v>2267</v>
@@ -35718,7 +35718,7 @@
         <v>0.0412637383917675</v>
       </c>
       <c r="E270" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F270" t="s">
         <v>2276</v>
@@ -37525,7 +37525,7 @@
         <v>42</v>
       </c>
       <c r="T287" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U287" t="n">
         <v>92532.2745098039</v>
@@ -37939,7 +37939,7 @@
         <v>35</v>
       </c>
       <c r="T291" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U291" t="n">
         <v>414179.411764706</v>
@@ -38095,7 +38095,7 @@
         <v>0.954203411581308</v>
       </c>
       <c r="D293" t="n">
-        <v>0.0468029766410784</v>
+        <v>0.0468029766410783</v>
       </c>
       <c r="E293" t="n">
         <v>0.385015325892463</v>
@@ -38705,7 +38705,7 @@
         <v>1.19638760298473</v>
       </c>
       <c r="D299" t="n">
-        <v>0.0483823662658333</v>
+        <v>0.0483823662658334</v>
       </c>
       <c r="E299" t="n">
         <v>0.387625187717942</v>
@@ -39121,7 +39121,7 @@
         <v>1.35134538902765</v>
       </c>
       <c r="D303" t="n">
-        <v>0.0486856279723761</v>
+        <v>0.0486856279723762</v>
       </c>
       <c r="E303" t="n">
         <v>0.387625187717942</v>
@@ -39327,7 +39327,7 @@
         <v>1.43659926223378</v>
       </c>
       <c r="D305" t="n">
-        <v>0.0493091279355316</v>
+        <v>0.0493091279355317</v>
       </c>
       <c r="E305" t="n">
         <v>0.387625187717942</v>
@@ -39887,7 +39887,7 @@
         <v>35</v>
       </c>
       <c r="T310" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U310" t="n">
         <v>177143.539215686</v>

</xml_diff>

<commit_message>
finsihed all correlation plots for fig 3
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/annot_results.xlsx
+++ b/Outputs/Annotation/annot_results.xlsx
@@ -8174,7 +8174,7 @@
         <v>0.0000000178519669484774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000406667807086316</v>
+        <v>0.0000406667807086315</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -8379,10 +8379,10 @@
         <v>1.50535400752026</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000475639853287726</v>
+        <v>0.0000475639853287725</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
@@ -8483,10 +8483,10 @@
         <v>1.80212684967551</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000499847719483915</v>
+        <v>0.0000499847719483916</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -8587,10 +8587,10 @@
         <v>2.09431049210052</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0000517922239009609</v>
+        <v>0.0000517922239009611</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F6" t="s">
         <v>90</v>
@@ -8794,7 +8794,7 @@
         <v>0.000110008275103165</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
@@ -8894,7 +8894,7 @@
         <v>0.000111361244672891</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F9" t="s">
         <v>122</v>
@@ -8998,7 +8998,7 @@
         <v>0.000112205604722291</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F10" t="s">
         <v>133</v>
@@ -9097,10 +9097,10 @@
         <v>1.04982890375572</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000126131019936541</v>
+        <v>0.000126131019936542</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0287326463415441</v>
+        <v>0.0287326463415442</v>
       </c>
       <c r="F11" t="s">
         <v>143</v>
@@ -9303,7 +9303,7 @@
         <v>0.986049090397621</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000192246012402053</v>
+        <v>0.000192246012402054</v>
       </c>
       <c r="E13" t="n">
         <v>0.032545879390594</v>
@@ -9717,7 +9717,7 @@
         <v>1.33076563688241</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000254639461413521</v>
+        <v>0.000254639461413522</v>
       </c>
       <c r="E17" t="n">
         <v>0.0362542933187501</v>
@@ -9928,7 +9928,7 @@
         <v>0.000380908914516266</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0482061392926696</v>
+        <v>0.0482061392926697</v>
       </c>
       <c r="F19" t="s">
         <v>219</v>
@@ -10131,7 +10131,7 @@
         <v>2.11985942237007</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000440559084185694</v>
+        <v>0.000440559084185693</v>
       </c>
       <c r="E21" t="n">
         <v>0.0501796796887505</v>
@@ -10233,7 +10233,7 @@
         <v>1.91995019137173</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000500571753448367</v>
+        <v>0.000500571753448369</v>
       </c>
       <c r="E22" t="n">
         <v>0.0521990821189653</v>
@@ -10335,7 +10335,7 @@
         <v>1.61125465202653</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000504117562167355</v>
+        <v>0.000504117562167356</v>
       </c>
       <c r="E23" t="n">
         <v>0.0521990821189653</v>
@@ -10439,7 +10439,7 @@
         <v>2.19572074738617</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000536816012583925</v>
+        <v>0.000536816012583926</v>
       </c>
       <c r="E24" t="n">
         <v>0.0531681250724427</v>
@@ -10849,7 +10849,7 @@
         <v>2.5917608012007</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000922568990829641</v>
+        <v>0.000922568990829643</v>
       </c>
       <c r="E28" t="n">
         <v>0.0764489881865432</v>
@@ -11060,7 +11060,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F30" t="s">
         <v>328</v>
@@ -11162,7 +11162,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F31" t="s">
         <v>328</v>
@@ -11264,7 +11264,7 @@
         <v>0.00105194943882193</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F32" t="s">
         <v>342</v>
@@ -11366,7 +11366,7 @@
         <v>0.00105453471953679</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F33" t="s">
         <v>350</v>
@@ -11468,7 +11468,7 @@
         <v>0.00108883939495889</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0775117544286356</v>
+        <v>0.0775117544286357</v>
       </c>
       <c r="F34" t="s">
         <v>361</v>
@@ -11572,7 +11572,7 @@
         <v>0.0013671855217853</v>
       </c>
       <c r="E35" t="n">
-        <v>0.094377230867482</v>
+        <v>0.0943772308674821</v>
       </c>
       <c r="F35" t="s">
         <v>371</v>
@@ -11673,7 +11673,7 @@
         <v>2.28004007337048</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00175062336032302</v>
+        <v>0.00175062336032303</v>
       </c>
       <c r="E36" t="n">
         <v>0.115407122551921</v>
@@ -11773,7 +11773,7 @@
         <v>2.22193178182585</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00177315596545971</v>
+        <v>0.00177315596545972</v>
       </c>
       <c r="E37" t="n">
         <v>0.115407122551921</v>
@@ -12805,7 +12805,7 @@
         <v>1.10076053003269</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00256069584580061</v>
+        <v>0.00256069584580062</v>
       </c>
       <c r="E47" t="n">
         <v>0.127772460423391</v>
@@ -12957,7 +12957,7 @@
         <v>35</v>
       </c>
       <c r="T48" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U48" t="n">
         <v>611583.803921569</v>
@@ -13115,7 +13115,7 @@
         <v>1.74722767046515</v>
       </c>
       <c r="D50" t="n">
-        <v>0.00283700757238659</v>
+        <v>0.0028370075723866</v>
       </c>
       <c r="E50" t="n">
         <v>0.134536691710072</v>
@@ -13525,7 +13525,7 @@
         <v>1.87754894817857</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0030861961631108</v>
+        <v>0.00308619616311079</v>
       </c>
       <c r="E54" t="n">
         <v>0.135199131914738</v>
@@ -14033,7 +14033,7 @@
         <v>1.5984185900808</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00369826788451144</v>
+        <v>0.00369826788451145</v>
       </c>
       <c r="E59" t="n">
         <v>0.146018369479691</v>
@@ -14354,7 +14354,7 @@
         <v>609</v>
       </c>
       <c r="G62" t="n">
-        <v>15.989438076772</v>
+        <v>15.9894380767719</v>
       </c>
       <c r="H62" t="n">
         <v>15.4535504246111</v>
@@ -14600,10 +14600,10 @@
         <v>100</v>
       </c>
       <c r="U64" t="n">
-        <v>639738.19047619</v>
+        <v>639738.190476191</v>
       </c>
       <c r="V64" t="n">
-        <v>639738.19047619</v>
+        <v>639738.190476191</v>
       </c>
       <c r="W64" t="s">
         <v>43</v>
@@ -14757,7 +14757,7 @@
         <v>-1.03719098907359</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00463820694388654</v>
+        <v>0.00463820694388655</v>
       </c>
       <c r="E66" t="n">
         <v>0.161109582380577</v>
@@ -15117,7 +15117,7 @@
         <v>35</v>
       </c>
       <c r="T69" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U69" t="n">
         <v>138049.460784314</v>
@@ -15171,7 +15171,7 @@
         <v>-1.09646153941116</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00480924126509184</v>
+        <v>0.00480924126509185</v>
       </c>
       <c r="E70" t="n">
         <v>0.161109582380577</v>
@@ -15273,7 +15273,7 @@
         <v>1.65173907709379</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00516491822274915</v>
+        <v>0.00516491822274916</v>
       </c>
       <c r="E71" t="n">
         <v>0.170517155238008</v>
@@ -15479,7 +15479,7 @@
         <v>1.54031082907751</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0054125978737031</v>
+        <v>0.00541259787370311</v>
       </c>
       <c r="E73" t="n">
         <v>0.173660534595714</v>
@@ -15683,10 +15683,10 @@
         <v>-1.43617464044618</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00610288959285423</v>
+        <v>0.00610288959285422</v>
       </c>
       <c r="E75" t="n">
-        <v>0.190443595787972</v>
+        <v>0.190443595787971</v>
       </c>
       <c r="F75" t="s">
         <v>730</v>
@@ -15785,7 +15785,7 @@
         <v>1.72026699754165</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00642796743910865</v>
+        <v>0.00642796743910863</v>
       </c>
       <c r="E76" t="n">
         <v>0.197877159814723</v>
@@ -15889,7 +15889,7 @@
         <v>0.697530163216005</v>
       </c>
       <c r="D77" t="n">
-        <v>0.00670714671808457</v>
+        <v>0.00670714671808456</v>
       </c>
       <c r="E77" t="n">
         <v>0.198403812483892</v>
@@ -15991,7 +15991,7 @@
         <v>0.963481828171481</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00698817479448876</v>
+        <v>0.00698817479448877</v>
       </c>
       <c r="E78" t="n">
         <v>0.198403812483892</v>
@@ -16095,7 +16095,7 @@
         <v>3.03596056752893</v>
       </c>
       <c r="D79" t="n">
-        <v>0.00703056100385651</v>
+        <v>0.0070305610038565</v>
       </c>
       <c r="E79" t="n">
         <v>0.198403812483892</v>
@@ -16303,7 +16303,7 @@
         <v>1.26212292928929</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00711076042683457</v>
+        <v>0.00711076042683458</v>
       </c>
       <c r="E81" t="n">
         <v>0.198403812483892</v>
@@ -16555,7 +16555,7 @@
         <v>35</v>
       </c>
       <c r="T83" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U83" t="n">
         <v>104827.980392157</v>
@@ -16713,7 +16713,7 @@
         <v>1.26366052895703</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00722893610015937</v>
+        <v>0.00722893610015938</v>
       </c>
       <c r="E85" t="n">
         <v>0.198403812483892</v>
@@ -16815,7 +16815,7 @@
         <v>1.99233523129815</v>
       </c>
       <c r="D86" t="n">
-        <v>0.00739475449660171</v>
+        <v>0.0073947544966017</v>
       </c>
       <c r="E86" t="n">
         <v>0.200538699324508</v>
@@ -17537,7 +17537,7 @@
         <v>2.51435325201981</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00884745745358603</v>
+        <v>0.00884745745358602</v>
       </c>
       <c r="E93" t="n">
         <v>0.219946192103018</v>
@@ -17847,10 +17847,10 @@
         <v>1.33902553078093</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0091210582025955</v>
+        <v>0.00912105820259549</v>
       </c>
       <c r="E96" t="n">
-        <v>0.221040112611836</v>
+        <v>0.221040112611835</v>
       </c>
       <c r="F96" t="s">
         <v>904</v>
@@ -18051,7 +18051,7 @@
         <v>1.76072590332704</v>
       </c>
       <c r="D98" t="n">
-        <v>0.00938134437347442</v>
+        <v>0.00938134437347441</v>
       </c>
       <c r="E98" t="n">
         <v>0.22261148419557</v>
@@ -18257,7 +18257,7 @@
         <v>1.82034483729149</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00972177970932418</v>
+        <v>0.00972177970932419</v>
       </c>
       <c r="E100" t="n">
         <v>0.225981777324903</v>
@@ -18359,7 +18359,7 @@
         <v>1.63103264825839</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0098435358015774</v>
+        <v>0.00984353580157741</v>
       </c>
       <c r="E101" t="n">
         <v>0.226500753090842</v>
@@ -19281,10 +19281,10 @@
         <v>0.626816037819076</v>
       </c>
       <c r="D110" t="n">
-        <v>0.0115503256732989</v>
+        <v>0.011550325673299</v>
       </c>
       <c r="E110" t="n">
-        <v>0.243626313738657</v>
+        <v>0.243626313738658</v>
       </c>
       <c r="F110" t="s">
         <v>1021</v>
@@ -20302,7 +20302,7 @@
         <v>0.0128191613675105</v>
       </c>
       <c r="E120" t="n">
-        <v>0.247474996569399</v>
+        <v>0.247474996569398</v>
       </c>
       <c r="F120" t="s">
         <v>1101</v>
@@ -20404,7 +20404,7 @@
         <v>0.0130184057604316</v>
       </c>
       <c r="E121" t="n">
-        <v>0.24920948169969</v>
+        <v>0.249209481699691</v>
       </c>
       <c r="F121" t="s">
         <v>1109</v>
@@ -20607,7 +20607,7 @@
         <v>2.41635984686688</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0135023421528919</v>
+        <v>0.0135023421528918</v>
       </c>
       <c r="E123" t="n">
         <v>0.254201119208989</v>
@@ -24027,7 +24027,7 @@
         <v>35</v>
       </c>
       <c r="T156" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U156" t="n">
         <v>320818.843137255</v>
@@ -24287,7 +24287,7 @@
         <v>2.09123850802625</v>
       </c>
       <c r="D159" t="n">
-        <v>0.019990741169975</v>
+        <v>0.0199907411699751</v>
       </c>
       <c r="E159" t="n">
         <v>0.290056741307027</v>
@@ -25011,7 +25011,7 @@
         <v>1.21762092344371</v>
       </c>
       <c r="D166" t="n">
-        <v>0.0210472208862264</v>
+        <v>0.0210472208862265</v>
       </c>
       <c r="E166" t="n">
         <v>0.292351031578194</v>
@@ -25523,7 +25523,7 @@
         <v>0.867853197341834</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0226620463765856</v>
+        <v>0.0226620463765855</v>
       </c>
       <c r="E171" t="n">
         <v>0.302772694851184</v>
@@ -25729,7 +25729,7 @@
         <v>0.78371578317638</v>
       </c>
       <c r="D173" t="n">
-        <v>0.022815822360676</v>
+        <v>0.0228158223606759</v>
       </c>
       <c r="E173" t="n">
         <v>0.302772694851184</v>
@@ -25983,7 +25983,7 @@
         <v>35</v>
       </c>
       <c r="T175" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U175" t="n">
         <v>14629.5392156863</v>
@@ -26761,7 +26761,7 @@
         <v>1.57761266392044</v>
       </c>
       <c r="D183" t="n">
-        <v>0.02456910025865</v>
+        <v>0.0245691002586501</v>
       </c>
       <c r="E183" t="n">
         <v>0.31093561327336</v>
@@ -26865,10 +26865,10 @@
         <v>0.27905489843125</v>
       </c>
       <c r="D184" t="n">
-        <v>0.024859450574423</v>
+        <v>0.0248594505744229</v>
       </c>
       <c r="E184" t="n">
-        <v>0.312871980157655</v>
+        <v>0.312871980157654</v>
       </c>
       <c r="F184" t="s">
         <v>1610</v>
@@ -27901,7 +27901,7 @@
         <v>1.25376454302494</v>
       </c>
       <c r="D194" t="n">
-        <v>0.0268198605739048</v>
+        <v>0.0268198605739047</v>
       </c>
       <c r="E194" t="n">
         <v>0.320208023246158</v>
@@ -28211,7 +28211,7 @@
         <v>0.934103101296284</v>
       </c>
       <c r="D197" t="n">
-        <v>0.0270112981520271</v>
+        <v>0.027011298152027</v>
       </c>
       <c r="E197" t="n">
         <v>0.320477797866238</v>
@@ -28420,7 +28420,7 @@
         <v>0.0276051011071821</v>
       </c>
       <c r="E199" t="n">
-        <v>0.324146496505984</v>
+        <v>0.324146496505983</v>
       </c>
       <c r="F199" t="s">
         <v>1725</v>
@@ -30573,7 +30573,7 @@
         <v>1.22119471051002</v>
       </c>
       <c r="D220" t="n">
-        <v>0.0313979597922135</v>
+        <v>0.0313979597922136</v>
       </c>
       <c r="E220" t="n">
         <v>0.334574251532132</v>
@@ -30782,7 +30782,7 @@
         <v>0.0318779053495754</v>
       </c>
       <c r="E222" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F222" t="s">
         <v>1908</v>
@@ -30881,10 +30881,10 @@
         <v>2.26264357683325</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0319603715053674</v>
+        <v>0.0319603715053673</v>
       </c>
       <c r="E223" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F223" t="s">
         <v>1918</v>
@@ -30986,7 +30986,7 @@
         <v>0.0320126471951682</v>
       </c>
       <c r="E224" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F224" t="s">
         <v>1925</v>
@@ -31397,7 +31397,7 @@
         <v>1.78887655907102</v>
       </c>
       <c r="D228" t="n">
-        <v>0.0337919159899818</v>
+        <v>0.0337919159899819</v>
       </c>
       <c r="E228" t="n">
         <v>0.344552495084485</v>
@@ -31415,7 +31415,7 @@
         <v>14.6473805435874</v>
       </c>
       <c r="J228" t="n">
-        <v>3.45545707860451</v>
+        <v>3.4554570786045</v>
       </c>
       <c r="K228" t="s">
         <v>1961</v>
@@ -31499,7 +31499,7 @@
         <v>0.99704828479797</v>
       </c>
       <c r="D229" t="n">
-        <v>0.0338290806249596</v>
+        <v>0.0338290806249597</v>
       </c>
       <c r="E229" t="n">
         <v>0.344552495084485</v>
@@ -32115,7 +32115,7 @@
         <v>0.345489069906911</v>
       </c>
       <c r="D235" t="n">
-        <v>0.0346714061628504</v>
+        <v>0.0346714061628505</v>
       </c>
       <c r="E235" t="n">
         <v>0.344552495084485</v>
@@ -32336,7 +32336,7 @@
         <v>16.7343818564733</v>
       </c>
       <c r="I237" t="n">
-        <v>16.33772736267</v>
+        <v>16.3377273626701</v>
       </c>
       <c r="J237" t="n">
         <v>1.36152590482721</v>
@@ -32425,7 +32425,7 @@
         <v>1.74087635676352</v>
       </c>
       <c r="D238" t="n">
-        <v>0.0350155554167379</v>
+        <v>0.0350155554167378</v>
       </c>
       <c r="E238" t="n">
         <v>0.344552495084485</v>
@@ -33449,7 +33449,7 @@
         <v>1.80708411033922</v>
       </c>
       <c r="D248" t="n">
-        <v>0.037846962738846</v>
+        <v>0.0378469627388461</v>
       </c>
       <c r="E248" t="n">
         <v>0.355763774130317</v>
@@ -34189,7 +34189,7 @@
         <v>27.2048783401882</v>
       </c>
       <c r="J255" t="n">
-        <v>2.160645201853</v>
+        <v>2.16064520185301</v>
       </c>
       <c r="K255" t="s">
         <v>2161</v>
@@ -34375,7 +34375,7 @@
         <v>1.27522696767494</v>
       </c>
       <c r="D257" t="n">
-        <v>0.0394247070068918</v>
+        <v>0.0394247070068917</v>
       </c>
       <c r="E257" t="n">
         <v>0.357433512293212</v>
@@ -35043,7 +35043,7 @@
         <v>35</v>
       </c>
       <c r="T263" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U263" t="n">
         <v>515977.68627451</v>
@@ -35145,7 +35145,7 @@
         <v>35</v>
       </c>
       <c r="T264" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U264" t="n">
         <v>515977.68627451</v>
@@ -35199,7 +35199,7 @@
         <v>0.961685940676187</v>
       </c>
       <c r="D265" t="n">
-        <v>0.0404195812337835</v>
+        <v>0.0404195812337836</v>
       </c>
       <c r="E265" t="n">
         <v>0.357456311668854</v>
@@ -35211,7 +35211,7 @@
         <v>28.0202647722528</v>
       </c>
       <c r="H265" t="n">
-        <v>28.981950712929</v>
+        <v>28.9819507129289</v>
       </c>
       <c r="I265" t="n">
         <v>28.1251759657811</v>
@@ -35410,7 +35410,7 @@
         <v>0.0408089847599079</v>
       </c>
       <c r="E267" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F267" t="s">
         <v>2252</v>
@@ -35512,7 +35512,7 @@
         <v>0.0410740982767807</v>
       </c>
       <c r="E268" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F268" t="s">
         <v>2259</v>
@@ -35614,7 +35614,7 @@
         <v>0.0411672875092047</v>
       </c>
       <c r="E269" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F269" t="s">
         <v>2267</v>
@@ -35718,7 +35718,7 @@
         <v>0.0412637383917675</v>
       </c>
       <c r="E270" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F270" t="s">
         <v>2276</v>
@@ -37525,7 +37525,7 @@
         <v>42</v>
       </c>
       <c r="T287" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U287" t="n">
         <v>92532.2745098039</v>
@@ -37939,7 +37939,7 @@
         <v>35</v>
       </c>
       <c r="T291" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U291" t="n">
         <v>414179.411764706</v>
@@ -38095,7 +38095,7 @@
         <v>0.954203411581308</v>
       </c>
       <c r="D293" t="n">
-        <v>0.0468029766410783</v>
+        <v>0.0468029766410784</v>
       </c>
       <c r="E293" t="n">
         <v>0.385015325892463</v>
@@ -38705,7 +38705,7 @@
         <v>1.19638760298473</v>
       </c>
       <c r="D299" t="n">
-        <v>0.0483823662658334</v>
+        <v>0.0483823662658333</v>
       </c>
       <c r="E299" t="n">
         <v>0.387625187717942</v>
@@ -39121,7 +39121,7 @@
         <v>1.35134538902765</v>
       </c>
       <c r="D303" t="n">
-        <v>0.0486856279723762</v>
+        <v>0.0486856279723761</v>
       </c>
       <c r="E303" t="n">
         <v>0.387625187717942</v>
@@ -39327,7 +39327,7 @@
         <v>1.43659926223378</v>
       </c>
       <c r="D305" t="n">
-        <v>0.0493091279355317</v>
+        <v>0.0493091279355316</v>
       </c>
       <c r="E305" t="n">
         <v>0.387625187717942</v>
@@ -39887,7 +39887,7 @@
         <v>35</v>
       </c>
       <c r="T310" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U310" t="n">
         <v>177143.539215686</v>

</xml_diff>

<commit_message>
updated data not shown
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/annot_results.xlsx
+++ b/Outputs/Annotation/annot_results.xlsx
@@ -8174,7 +8174,7 @@
         <v>0.0000000178519669484774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000406667807086315</v>
+        <v>0.0000406667807086316</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -8379,10 +8379,10 @@
         <v>1.50535400752026</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000475639853287725</v>
+        <v>0.0000475639853287726</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
@@ -8483,10 +8483,10 @@
         <v>1.80212684967551</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000499847719483916</v>
+        <v>0.0000499847719483915</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -8587,10 +8587,10 @@
         <v>2.09431049210052</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0000517922239009611</v>
+        <v>0.0000517922239009609</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0235965372092779</v>
+        <v>0.0235965372092778</v>
       </c>
       <c r="F6" t="s">
         <v>90</v>
@@ -8794,7 +8794,7 @@
         <v>0.000110008275103165</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
@@ -8894,7 +8894,7 @@
         <v>0.000111361244672891</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F9" t="s">
         <v>122</v>
@@ -8998,7 +8998,7 @@
         <v>0.000112205604722291</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0284004852841532</v>
+        <v>0.0284004852841531</v>
       </c>
       <c r="F10" t="s">
         <v>133</v>
@@ -9097,10 +9097,10 @@
         <v>1.04982890375572</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000126131019936542</v>
+        <v>0.000126131019936541</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0287326463415442</v>
+        <v>0.0287326463415441</v>
       </c>
       <c r="F11" t="s">
         <v>143</v>
@@ -9303,7 +9303,7 @@
         <v>0.986049090397621</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000192246012402054</v>
+        <v>0.000192246012402053</v>
       </c>
       <c r="E13" t="n">
         <v>0.032545879390594</v>
@@ -9717,7 +9717,7 @@
         <v>1.33076563688241</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000254639461413522</v>
+        <v>0.000254639461413521</v>
       </c>
       <c r="E17" t="n">
         <v>0.0362542933187501</v>
@@ -9928,7 +9928,7 @@
         <v>0.000380908914516266</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0482061392926697</v>
+        <v>0.0482061392926696</v>
       </c>
       <c r="F19" t="s">
         <v>219</v>
@@ -10131,7 +10131,7 @@
         <v>2.11985942237007</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000440559084185693</v>
+        <v>0.000440559084185694</v>
       </c>
       <c r="E21" t="n">
         <v>0.0501796796887505</v>
@@ -10233,7 +10233,7 @@
         <v>1.91995019137173</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000500571753448369</v>
+        <v>0.000500571753448367</v>
       </c>
       <c r="E22" t="n">
         <v>0.0521990821189653</v>
@@ -10335,7 +10335,7 @@
         <v>1.61125465202653</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000504117562167356</v>
+        <v>0.000504117562167355</v>
       </c>
       <c r="E23" t="n">
         <v>0.0521990821189653</v>
@@ -10439,7 +10439,7 @@
         <v>2.19572074738617</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000536816012583926</v>
+        <v>0.000536816012583925</v>
       </c>
       <c r="E24" t="n">
         <v>0.0531681250724427</v>
@@ -10849,7 +10849,7 @@
         <v>2.5917608012007</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000922568990829643</v>
+        <v>0.000922568990829641</v>
       </c>
       <c r="E28" t="n">
         <v>0.0764489881865432</v>
@@ -11060,7 +11060,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F30" t="s">
         <v>328</v>
@@ -11162,7 +11162,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F31" t="s">
         <v>328</v>
@@ -11264,7 +11264,7 @@
         <v>0.00105194943882193</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F32" t="s">
         <v>342</v>
@@ -11366,7 +11366,7 @@
         <v>0.00105453471953679</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0774912932614457</v>
+        <v>0.0774912932614456</v>
       </c>
       <c r="F33" t="s">
         <v>350</v>
@@ -11468,7 +11468,7 @@
         <v>0.00108883939495889</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0775117544286357</v>
+        <v>0.0775117544286356</v>
       </c>
       <c r="F34" t="s">
         <v>361</v>
@@ -11572,7 +11572,7 @@
         <v>0.0013671855217853</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0943772308674821</v>
+        <v>0.094377230867482</v>
       </c>
       <c r="F35" t="s">
         <v>371</v>
@@ -11673,7 +11673,7 @@
         <v>2.28004007337048</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00175062336032303</v>
+        <v>0.00175062336032302</v>
       </c>
       <c r="E36" t="n">
         <v>0.115407122551921</v>
@@ -11773,7 +11773,7 @@
         <v>2.22193178182585</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00177315596545972</v>
+        <v>0.00177315596545971</v>
       </c>
       <c r="E37" t="n">
         <v>0.115407122551921</v>
@@ -12805,7 +12805,7 @@
         <v>1.10076053003269</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00256069584580062</v>
+        <v>0.00256069584580061</v>
       </c>
       <c r="E47" t="n">
         <v>0.127772460423391</v>
@@ -12957,7 +12957,7 @@
         <v>35</v>
       </c>
       <c r="T48" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U48" t="n">
         <v>611583.803921569</v>
@@ -13115,7 +13115,7 @@
         <v>1.74722767046515</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0028370075723866</v>
+        <v>0.00283700757238659</v>
       </c>
       <c r="E50" t="n">
         <v>0.134536691710072</v>
@@ -13525,7 +13525,7 @@
         <v>1.87754894817857</v>
       </c>
       <c r="D54" t="n">
-        <v>0.00308619616311079</v>
+        <v>0.0030861961631108</v>
       </c>
       <c r="E54" t="n">
         <v>0.135199131914738</v>
@@ -14033,7 +14033,7 @@
         <v>1.5984185900808</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00369826788451145</v>
+        <v>0.00369826788451144</v>
       </c>
       <c r="E59" t="n">
         <v>0.146018369479691</v>
@@ -14354,7 +14354,7 @@
         <v>609</v>
       </c>
       <c r="G62" t="n">
-        <v>15.9894380767719</v>
+        <v>15.989438076772</v>
       </c>
       <c r="H62" t="n">
         <v>15.4535504246111</v>
@@ -14600,10 +14600,10 @@
         <v>100</v>
       </c>
       <c r="U64" t="n">
-        <v>639738.190476191</v>
+        <v>639738.19047619</v>
       </c>
       <c r="V64" t="n">
-        <v>639738.190476191</v>
+        <v>639738.19047619</v>
       </c>
       <c r="W64" t="s">
         <v>43</v>
@@ -14757,7 +14757,7 @@
         <v>-1.03719098907359</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00463820694388655</v>
+        <v>0.00463820694388654</v>
       </c>
       <c r="E66" t="n">
         <v>0.161109582380577</v>
@@ -15117,7 +15117,7 @@
         <v>35</v>
       </c>
       <c r="T69" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U69" t="n">
         <v>138049.460784314</v>
@@ -15171,7 +15171,7 @@
         <v>-1.09646153941116</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00480924126509185</v>
+        <v>0.00480924126509184</v>
       </c>
       <c r="E70" t="n">
         <v>0.161109582380577</v>
@@ -15273,7 +15273,7 @@
         <v>1.65173907709379</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00516491822274916</v>
+        <v>0.00516491822274915</v>
       </c>
       <c r="E71" t="n">
         <v>0.170517155238008</v>
@@ -15479,7 +15479,7 @@
         <v>1.54031082907751</v>
       </c>
       <c r="D73" t="n">
-        <v>0.00541259787370311</v>
+        <v>0.0054125978737031</v>
       </c>
       <c r="E73" t="n">
         <v>0.173660534595714</v>
@@ -15683,10 +15683,10 @@
         <v>-1.43617464044618</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00610288959285422</v>
+        <v>0.00610288959285423</v>
       </c>
       <c r="E75" t="n">
-        <v>0.190443595787971</v>
+        <v>0.190443595787972</v>
       </c>
       <c r="F75" t="s">
         <v>730</v>
@@ -15785,7 +15785,7 @@
         <v>1.72026699754165</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00642796743910863</v>
+        <v>0.00642796743910865</v>
       </c>
       <c r="E76" t="n">
         <v>0.197877159814723</v>
@@ -15889,7 +15889,7 @@
         <v>0.697530163216005</v>
       </c>
       <c r="D77" t="n">
-        <v>0.00670714671808456</v>
+        <v>0.00670714671808457</v>
       </c>
       <c r="E77" t="n">
         <v>0.198403812483892</v>
@@ -15991,7 +15991,7 @@
         <v>0.963481828171481</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00698817479448877</v>
+        <v>0.00698817479448876</v>
       </c>
       <c r="E78" t="n">
         <v>0.198403812483892</v>
@@ -16095,7 +16095,7 @@
         <v>3.03596056752893</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0070305610038565</v>
+        <v>0.00703056100385651</v>
       </c>
       <c r="E79" t="n">
         <v>0.198403812483892</v>
@@ -16303,7 +16303,7 @@
         <v>1.26212292928929</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00711076042683458</v>
+        <v>0.00711076042683457</v>
       </c>
       <c r="E81" t="n">
         <v>0.198403812483892</v>
@@ -16555,7 +16555,7 @@
         <v>35</v>
       </c>
       <c r="T83" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U83" t="n">
         <v>104827.980392157</v>
@@ -16713,7 +16713,7 @@
         <v>1.26366052895703</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00722893610015938</v>
+        <v>0.00722893610015937</v>
       </c>
       <c r="E85" t="n">
         <v>0.198403812483892</v>
@@ -16815,7 +16815,7 @@
         <v>1.99233523129815</v>
       </c>
       <c r="D86" t="n">
-        <v>0.0073947544966017</v>
+        <v>0.00739475449660171</v>
       </c>
       <c r="E86" t="n">
         <v>0.200538699324508</v>
@@ -17537,7 +17537,7 @@
         <v>2.51435325201981</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00884745745358602</v>
+        <v>0.00884745745358603</v>
       </c>
       <c r="E93" t="n">
         <v>0.219946192103018</v>
@@ -17847,10 +17847,10 @@
         <v>1.33902553078093</v>
       </c>
       <c r="D96" t="n">
-        <v>0.00912105820259549</v>
+        <v>0.0091210582025955</v>
       </c>
       <c r="E96" t="n">
-        <v>0.221040112611835</v>
+        <v>0.221040112611836</v>
       </c>
       <c r="F96" t="s">
         <v>904</v>
@@ -18051,7 +18051,7 @@
         <v>1.76072590332704</v>
       </c>
       <c r="D98" t="n">
-        <v>0.00938134437347441</v>
+        <v>0.00938134437347442</v>
       </c>
       <c r="E98" t="n">
         <v>0.22261148419557</v>
@@ -18257,7 +18257,7 @@
         <v>1.82034483729149</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00972177970932419</v>
+        <v>0.00972177970932418</v>
       </c>
       <c r="E100" t="n">
         <v>0.225981777324903</v>
@@ -18359,7 +18359,7 @@
         <v>1.63103264825839</v>
       </c>
       <c r="D101" t="n">
-        <v>0.00984353580157741</v>
+        <v>0.0098435358015774</v>
       </c>
       <c r="E101" t="n">
         <v>0.226500753090842</v>
@@ -19281,10 +19281,10 @@
         <v>0.626816037819076</v>
       </c>
       <c r="D110" t="n">
-        <v>0.011550325673299</v>
+        <v>0.0115503256732989</v>
       </c>
       <c r="E110" t="n">
-        <v>0.243626313738658</v>
+        <v>0.243626313738657</v>
       </c>
       <c r="F110" t="s">
         <v>1021</v>
@@ -20302,7 +20302,7 @@
         <v>0.0128191613675105</v>
       </c>
       <c r="E120" t="n">
-        <v>0.247474996569398</v>
+        <v>0.247474996569399</v>
       </c>
       <c r="F120" t="s">
         <v>1101</v>
@@ -20404,7 +20404,7 @@
         <v>0.0130184057604316</v>
       </c>
       <c r="E121" t="n">
-        <v>0.249209481699691</v>
+        <v>0.24920948169969</v>
       </c>
       <c r="F121" t="s">
         <v>1109</v>
@@ -20607,7 +20607,7 @@
         <v>2.41635984686688</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0135023421528918</v>
+        <v>0.0135023421528919</v>
       </c>
       <c r="E123" t="n">
         <v>0.254201119208989</v>
@@ -24027,7 +24027,7 @@
         <v>35</v>
       </c>
       <c r="T156" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U156" t="n">
         <v>320818.843137255</v>
@@ -24287,7 +24287,7 @@
         <v>2.09123850802625</v>
       </c>
       <c r="D159" t="n">
-        <v>0.0199907411699751</v>
+        <v>0.019990741169975</v>
       </c>
       <c r="E159" t="n">
         <v>0.290056741307027</v>
@@ -25011,7 +25011,7 @@
         <v>1.21762092344371</v>
       </c>
       <c r="D166" t="n">
-        <v>0.0210472208862265</v>
+        <v>0.0210472208862264</v>
       </c>
       <c r="E166" t="n">
         <v>0.292351031578194</v>
@@ -25523,7 +25523,7 @@
         <v>0.867853197341834</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0226620463765855</v>
+        <v>0.0226620463765856</v>
       </c>
       <c r="E171" t="n">
         <v>0.302772694851184</v>
@@ -25729,7 +25729,7 @@
         <v>0.78371578317638</v>
       </c>
       <c r="D173" t="n">
-        <v>0.0228158223606759</v>
+        <v>0.022815822360676</v>
       </c>
       <c r="E173" t="n">
         <v>0.302772694851184</v>
@@ -25983,7 +25983,7 @@
         <v>35</v>
       </c>
       <c r="T175" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U175" t="n">
         <v>14629.5392156863</v>
@@ -26761,7 +26761,7 @@
         <v>1.57761266392044</v>
       </c>
       <c r="D183" t="n">
-        <v>0.0245691002586501</v>
+        <v>0.02456910025865</v>
       </c>
       <c r="E183" t="n">
         <v>0.31093561327336</v>
@@ -26865,10 +26865,10 @@
         <v>0.27905489843125</v>
       </c>
       <c r="D184" t="n">
-        <v>0.0248594505744229</v>
+        <v>0.024859450574423</v>
       </c>
       <c r="E184" t="n">
-        <v>0.312871980157654</v>
+        <v>0.312871980157655</v>
       </c>
       <c r="F184" t="s">
         <v>1610</v>
@@ -27901,7 +27901,7 @@
         <v>1.25376454302494</v>
       </c>
       <c r="D194" t="n">
-        <v>0.0268198605739047</v>
+        <v>0.0268198605739048</v>
       </c>
       <c r="E194" t="n">
         <v>0.320208023246158</v>
@@ -28211,7 +28211,7 @@
         <v>0.934103101296284</v>
       </c>
       <c r="D197" t="n">
-        <v>0.027011298152027</v>
+        <v>0.0270112981520271</v>
       </c>
       <c r="E197" t="n">
         <v>0.320477797866238</v>
@@ -28420,7 +28420,7 @@
         <v>0.0276051011071821</v>
       </c>
       <c r="E199" t="n">
-        <v>0.324146496505983</v>
+        <v>0.324146496505984</v>
       </c>
       <c r="F199" t="s">
         <v>1725</v>
@@ -30573,7 +30573,7 @@
         <v>1.22119471051002</v>
       </c>
       <c r="D220" t="n">
-        <v>0.0313979597922136</v>
+        <v>0.0313979597922135</v>
       </c>
       <c r="E220" t="n">
         <v>0.334574251532132</v>
@@ -30782,7 +30782,7 @@
         <v>0.0318779053495754</v>
       </c>
       <c r="E222" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F222" t="s">
         <v>1908</v>
@@ -30881,10 +30881,10 @@
         <v>2.26264357683325</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0319603715053673</v>
+        <v>0.0319603715053674</v>
       </c>
       <c r="E223" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F223" t="s">
         <v>1918</v>
@@ -30986,7 +30986,7 @@
         <v>0.0320126471951682</v>
       </c>
       <c r="E224" t="n">
-        <v>0.33605903368937</v>
+        <v>0.336059033689369</v>
       </c>
       <c r="F224" t="s">
         <v>1925</v>
@@ -31397,7 +31397,7 @@
         <v>1.78887655907102</v>
       </c>
       <c r="D228" t="n">
-        <v>0.0337919159899819</v>
+        <v>0.0337919159899818</v>
       </c>
       <c r="E228" t="n">
         <v>0.344552495084485</v>
@@ -31415,7 +31415,7 @@
         <v>14.6473805435874</v>
       </c>
       <c r="J228" t="n">
-        <v>3.4554570786045</v>
+        <v>3.45545707860451</v>
       </c>
       <c r="K228" t="s">
         <v>1961</v>
@@ -31499,7 +31499,7 @@
         <v>0.99704828479797</v>
       </c>
       <c r="D229" t="n">
-        <v>0.0338290806249597</v>
+        <v>0.0338290806249596</v>
       </c>
       <c r="E229" t="n">
         <v>0.344552495084485</v>
@@ -32115,7 +32115,7 @@
         <v>0.345489069906911</v>
       </c>
       <c r="D235" t="n">
-        <v>0.0346714061628505</v>
+        <v>0.0346714061628504</v>
       </c>
       <c r="E235" t="n">
         <v>0.344552495084485</v>
@@ -32336,7 +32336,7 @@
         <v>16.7343818564733</v>
       </c>
       <c r="I237" t="n">
-        <v>16.3377273626701</v>
+        <v>16.33772736267</v>
       </c>
       <c r="J237" t="n">
         <v>1.36152590482721</v>
@@ -32425,7 +32425,7 @@
         <v>1.74087635676352</v>
       </c>
       <c r="D238" t="n">
-        <v>0.0350155554167378</v>
+        <v>0.0350155554167379</v>
       </c>
       <c r="E238" t="n">
         <v>0.344552495084485</v>
@@ -33449,7 +33449,7 @@
         <v>1.80708411033922</v>
       </c>
       <c r="D248" t="n">
-        <v>0.0378469627388461</v>
+        <v>0.037846962738846</v>
       </c>
       <c r="E248" t="n">
         <v>0.355763774130317</v>
@@ -34189,7 +34189,7 @@
         <v>27.2048783401882</v>
       </c>
       <c r="J255" t="n">
-        <v>2.16064520185301</v>
+        <v>2.160645201853</v>
       </c>
       <c r="K255" t="s">
         <v>2161</v>
@@ -34375,7 +34375,7 @@
         <v>1.27522696767494</v>
       </c>
       <c r="D257" t="n">
-        <v>0.0394247070068917</v>
+        <v>0.0394247070068918</v>
       </c>
       <c r="E257" t="n">
         <v>0.357433512293212</v>
@@ -35043,7 +35043,7 @@
         <v>35</v>
       </c>
       <c r="T263" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U263" t="n">
         <v>515977.68627451</v>
@@ -35145,7 +35145,7 @@
         <v>35</v>
       </c>
       <c r="T264" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U264" t="n">
         <v>515977.68627451</v>
@@ -35199,7 +35199,7 @@
         <v>0.961685940676187</v>
       </c>
       <c r="D265" t="n">
-        <v>0.0404195812337836</v>
+        <v>0.0404195812337835</v>
       </c>
       <c r="E265" t="n">
         <v>0.357456311668854</v>
@@ -35211,7 +35211,7 @@
         <v>28.0202647722528</v>
       </c>
       <c r="H265" t="n">
-        <v>28.9819507129289</v>
+        <v>28.981950712929</v>
       </c>
       <c r="I265" t="n">
         <v>28.1251759657811</v>
@@ -35410,7 +35410,7 @@
         <v>0.0408089847599079</v>
       </c>
       <c r="E267" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F267" t="s">
         <v>2252</v>
@@ -35512,7 +35512,7 @@
         <v>0.0410740982767807</v>
       </c>
       <c r="E268" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F268" t="s">
         <v>2259</v>
@@ -35614,7 +35614,7 @@
         <v>0.0411672875092047</v>
       </c>
       <c r="E269" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F269" t="s">
         <v>2267</v>
@@ -35718,7 +35718,7 @@
         <v>0.0412637383917675</v>
       </c>
       <c r="E270" t="n">
-        <v>0.358774030749795</v>
+        <v>0.358774030749796</v>
       </c>
       <c r="F270" t="s">
         <v>2276</v>
@@ -37525,7 +37525,7 @@
         <v>42</v>
       </c>
       <c r="T287" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U287" t="n">
         <v>92532.2745098039</v>
@@ -37939,7 +37939,7 @@
         <v>35</v>
       </c>
       <c r="T291" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U291" t="n">
         <v>414179.411764706</v>
@@ -38095,7 +38095,7 @@
         <v>0.954203411581308</v>
       </c>
       <c r="D293" t="n">
-        <v>0.0468029766410784</v>
+        <v>0.0468029766410783</v>
       </c>
       <c r="E293" t="n">
         <v>0.385015325892463</v>
@@ -38705,7 +38705,7 @@
         <v>1.19638760298473</v>
       </c>
       <c r="D299" t="n">
-        <v>0.0483823662658333</v>
+        <v>0.0483823662658334</v>
       </c>
       <c r="E299" t="n">
         <v>0.387625187717942</v>
@@ -39121,7 +39121,7 @@
         <v>1.35134538902765</v>
       </c>
       <c r="D303" t="n">
-        <v>0.0486856279723761</v>
+        <v>0.0486856279723762</v>
       </c>
       <c r="E303" t="n">
         <v>0.387625187717942</v>
@@ -39327,7 +39327,7 @@
         <v>1.43659926223378</v>
       </c>
       <c r="D305" t="n">
-        <v>0.0493091279355316</v>
+        <v>0.0493091279355317</v>
       </c>
       <c r="E305" t="n">
         <v>0.387625187717942</v>
@@ -39887,7 +39887,7 @@
         <v>35</v>
       </c>
       <c r="T310" t="n">
-        <v>80.9523809523809</v>
+        <v>80.952380952381</v>
       </c>
       <c r="U310" t="n">
         <v>177143.539215686</v>

</xml_diff>

<commit_message>
finished adding heatmap to figure 1, ran
</commit_message>
<xml_diff>
--- a/Outputs/Annotation/annot_results.xlsx
+++ b/Outputs/Annotation/annot_results.xlsx
@@ -8174,7 +8174,7 @@
         <v>0.0000000178519669484774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000406667807086316</v>
+        <v>0.0000406667807086315</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -8379,10 +8379,10 @@
         <v>1.50535400752026</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0000475639853287726</v>
+        <v>0.0000475639853287725</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
@@ -8483,10 +8483,10 @@
         <v>1.80212684967551</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0000499847719483915</v>
+        <v>0.0000499847719483916</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F5" t="s">
         <v>77</v>
@@ -8587,10 +8587,10 @@
         <v>2.09431049210052</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0000517922239009609</v>
+        <v>0.0000517922239009611</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0235965372092778</v>
+        <v>0.0235965372092779</v>
       </c>
       <c r="F6" t="s">
         <v>90</v>
@@ -8794,7 +8794,7 @@
         <v>0.000110008275103165</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F8" t="s">
         <v>112</v>
@@ -8894,7 +8894,7 @@
         <v>0.000111361244672891</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F9" t="s">
         <v>122</v>
@@ -8998,7 +8998,7 @@
         <v>0.000112205604722291</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0284004852841531</v>
+        <v>0.0284004852841532</v>
       </c>
       <c r="F10" t="s">
         <v>133</v>
@@ -9097,10 +9097,10 @@
         <v>1.04982890375572</v>
       </c>
       <c r="D11" t="n">
-        <v>0.000126131019936541</v>
+        <v>0.000126131019936542</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0287326463415441</v>
+        <v>0.0287326463415442</v>
       </c>
       <c r="F11" t="s">
         <v>143</v>
@@ -9303,7 +9303,7 @@
         <v>0.986049090397621</v>
       </c>
       <c r="D13" t="n">
-        <v>0.000192246012402053</v>
+        <v>0.000192246012402054</v>
       </c>
       <c r="E13" t="n">
         <v>0.032545879390594</v>
@@ -9717,7 +9717,7 @@
         <v>1.33076563688241</v>
       </c>
       <c r="D17" t="n">
-        <v>0.000254639461413521</v>
+        <v>0.000254639461413522</v>
       </c>
       <c r="E17" t="n">
         <v>0.0362542933187501</v>
@@ -9928,7 +9928,7 @@
         <v>0.000380908914516266</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0482061392926696</v>
+        <v>0.0482061392926697</v>
       </c>
       <c r="F19" t="s">
         <v>219</v>
@@ -10131,7 +10131,7 @@
         <v>2.11985942237007</v>
       </c>
       <c r="D21" t="n">
-        <v>0.000440559084185694</v>
+        <v>0.000440559084185693</v>
       </c>
       <c r="E21" t="n">
         <v>0.0501796796887505</v>
@@ -10233,7 +10233,7 @@
         <v>1.91995019137173</v>
       </c>
       <c r="D22" t="n">
-        <v>0.000500571753448367</v>
+        <v>0.000500571753448369</v>
       </c>
       <c r="E22" t="n">
         <v>0.0521990821189653</v>
@@ -10335,7 +10335,7 @@
         <v>1.61125465202653</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000504117562167355</v>
+        <v>0.000504117562167356</v>
       </c>
       <c r="E23" t="n">
         <v>0.0521990821189653</v>
@@ -10439,7 +10439,7 @@
         <v>2.19572074738617</v>
       </c>
       <c r="D24" t="n">
-        <v>0.000536816012583925</v>
+        <v>0.000536816012583926</v>
       </c>
       <c r="E24" t="n">
         <v>0.0531681250724427</v>
@@ -10849,7 +10849,7 @@
         <v>2.5917608012007</v>
       </c>
       <c r="D28" t="n">
-        <v>0.000922568990829641</v>
+        <v>0.000922568990829643</v>
       </c>
       <c r="E28" t="n">
         <v>0.0764489881865432</v>
@@ -11060,7 +11060,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F30" t="s">
         <v>328</v>
@@ -11162,7 +11162,7 @@
         <v>0.00101245070716733</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F31" t="s">
         <v>328</v>
@@ -11264,7 +11264,7 @@
         <v>0.00105194943882193</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F32" t="s">
         <v>342</v>
@@ -11366,7 +11366,7 @@
         <v>0.00105453471953679</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0774912932614456</v>
+        <v>0.0774912932614457</v>
       </c>
       <c r="F33" t="s">
         <v>350</v>
@@ -11468,7 +11468,7 @@
         <v>0.00108883939495889</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0775117544286356</v>
+        <v>0.0775117544286357</v>
       </c>
       <c r="F34" t="s">
         <v>361</v>
@@ -11572,7 +11572,7 @@
         <v>0.0013671855217853</v>
       </c>
       <c r="E35" t="n">
-        <v>0.094377230867482</v>
+        <v>0.0943772308674821</v>
       </c>
       <c r="F35" t="s">
         <v>371</v>
@@ -11673,7 +11673,7 @@
         <v>2.28004007337048</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00175062336032302</v>
+        <v>0.00175062336032303</v>
       </c>
       <c r="E36" t="n">
         <v>0.115407122551921</v>
@@ -11773,7 +11773,7 @@
         <v>2.22193178182585</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00177315596545971</v>
+        <v>0.00177315596545972</v>
       </c>
       <c r="E37" t="n">
         <v>0.115407122551921</v>
@@ -12805,7 +12805,7 @@
         <v>1.10076053003269</v>
       </c>
       <c r="D47" t="n">
-        <v>0.00256069584580061</v>
+        <v>0.00256069584580062</v>
       </c>
       <c r="E47" t="n">
         <v>0.127772460423391</v>
@@ -12957,7 +12957,7 @@
         <v>35</v>
       </c>
       <c r="T48" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U48" t="n">
         <v>611583.803921569</v>
@@ -13115,7 +13115,7 @@
         <v>1.74722767046515</v>
       </c>
       <c r="D50" t="n">
-        <v>0.00283700757238659</v>
+        <v>0.0028370075723866</v>
       </c>
       <c r="E50" t="n">
         <v>0.134536691710072</v>
@@ -13525,7 +13525,7 @@
         <v>1.87754894817857</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0030861961631108</v>
+        <v>0.00308619616311079</v>
       </c>
       <c r="E54" t="n">
         <v>0.135199131914738</v>
@@ -14033,7 +14033,7 @@
         <v>1.5984185900808</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00369826788451144</v>
+        <v>0.00369826788451145</v>
       </c>
       <c r="E59" t="n">
         <v>0.146018369479691</v>
@@ -14354,7 +14354,7 @@
         <v>609</v>
       </c>
       <c r="G62" t="n">
-        <v>15.989438076772</v>
+        <v>15.9894380767719</v>
       </c>
       <c r="H62" t="n">
         <v>15.4535504246111</v>
@@ -14600,10 +14600,10 @@
         <v>100</v>
       </c>
       <c r="U64" t="n">
-        <v>639738.19047619</v>
+        <v>639738.190476191</v>
       </c>
       <c r="V64" t="n">
-        <v>639738.19047619</v>
+        <v>639738.190476191</v>
       </c>
       <c r="W64" t="s">
         <v>43</v>
@@ -14757,7 +14757,7 @@
         <v>-1.03719098907359</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00463820694388654</v>
+        <v>0.00463820694388655</v>
       </c>
       <c r="E66" t="n">
         <v>0.161109582380577</v>
@@ -15117,7 +15117,7 @@
         <v>35</v>
       </c>
       <c r="T69" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U69" t="n">
         <v>138049.460784314</v>
@@ -15171,7 +15171,7 @@
         <v>-1.09646153941116</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00480924126509184</v>
+        <v>0.00480924126509185</v>
       </c>
       <c r="E70" t="n">
         <v>0.161109582380577</v>
@@ -15273,7 +15273,7 @@
         <v>1.65173907709379</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00516491822274915</v>
+        <v>0.00516491822274916</v>
       </c>
       <c r="E71" t="n">
         <v>0.170517155238008</v>
@@ -15479,7 +15479,7 @@
         <v>1.54031082907751</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0054125978737031</v>
+        <v>0.00541259787370311</v>
       </c>
       <c r="E73" t="n">
         <v>0.173660534595714</v>
@@ -15683,10 +15683,10 @@
         <v>-1.43617464044618</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00610288959285423</v>
+        <v>0.00610288959285422</v>
       </c>
       <c r="E75" t="n">
-        <v>0.190443595787972</v>
+        <v>0.190443595787971</v>
       </c>
       <c r="F75" t="s">
         <v>730</v>
@@ -15785,7 +15785,7 @@
         <v>1.72026699754165</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00642796743910865</v>
+        <v>0.00642796743910863</v>
       </c>
       <c r="E76" t="n">
         <v>0.197877159814723</v>
@@ -15889,7 +15889,7 @@
         <v>0.697530163216005</v>
       </c>
       <c r="D77" t="n">
-        <v>0.00670714671808457</v>
+        <v>0.00670714671808456</v>
       </c>
       <c r="E77" t="n">
         <v>0.198403812483892</v>
@@ -15991,7 +15991,7 @@
         <v>0.963481828171481</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00698817479448876</v>
+        <v>0.00698817479448877</v>
       </c>
       <c r="E78" t="n">
         <v>0.198403812483892</v>
@@ -16095,7 +16095,7 @@
         <v>3.03596056752893</v>
       </c>
       <c r="D79" t="n">
-        <v>0.00703056100385651</v>
+        <v>0.0070305610038565</v>
       </c>
       <c r="E79" t="n">
         <v>0.198403812483892</v>
@@ -16303,7 +16303,7 @@
         <v>1.26212292928929</v>
       </c>
       <c r="D81" t="n">
-        <v>0.00711076042683457</v>
+        <v>0.00711076042683458</v>
       </c>
       <c r="E81" t="n">
         <v>0.198403812483892</v>
@@ -16555,7 +16555,7 @@
         <v>35</v>
       </c>
       <c r="T83" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U83" t="n">
         <v>104827.980392157</v>
@@ -16713,7 +16713,7 @@
         <v>1.26366052895703</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00722893610015937</v>
+        <v>0.00722893610015938</v>
       </c>
       <c r="E85" t="n">
         <v>0.198403812483892</v>
@@ -16815,7 +16815,7 @@
         <v>1.99233523129815</v>
       </c>
       <c r="D86" t="n">
-        <v>0.00739475449660171</v>
+        <v>0.0073947544966017</v>
       </c>
       <c r="E86" t="n">
         <v>0.200538699324508</v>
@@ -17537,7 +17537,7 @@
         <v>2.51435325201981</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00884745745358603</v>
+        <v>0.00884745745358602</v>
       </c>
       <c r="E93" t="n">
         <v>0.219946192103018</v>
@@ -17847,10 +17847,10 @@
         <v>1.33902553078093</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0091210582025955</v>
+        <v>0.00912105820259549</v>
       </c>
       <c r="E96" t="n">
-        <v>0.221040112611836</v>
+        <v>0.221040112611835</v>
       </c>
       <c r="F96" t="s">
         <v>904</v>
@@ -18051,7 +18051,7 @@
         <v>1.76072590332704</v>
       </c>
       <c r="D98" t="n">
-        <v>0.00938134437347442</v>
+        <v>0.00938134437347441</v>
       </c>
       <c r="E98" t="n">
         <v>0.22261148419557</v>
@@ -18257,7 +18257,7 @@
         <v>1.82034483729149</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00972177970932418</v>
+        <v>0.00972177970932419</v>
       </c>
       <c r="E100" t="n">
         <v>0.225981777324903</v>
@@ -18359,7 +18359,7 @@
         <v>1.63103264825839</v>
       </c>
       <c r="D101" t="n">
-        <v>0.0098435358015774</v>
+        <v>0.00984353580157741</v>
       </c>
       <c r="E101" t="n">
         <v>0.226500753090842</v>
@@ -19281,10 +19281,10 @@
         <v>0.626816037819076</v>
       </c>
       <c r="D110" t="n">
-        <v>0.0115503256732989</v>
+        <v>0.011550325673299</v>
       </c>
       <c r="E110" t="n">
-        <v>0.243626313738657</v>
+        <v>0.243626313738658</v>
       </c>
       <c r="F110" t="s">
         <v>1021</v>
@@ -20302,7 +20302,7 @@
         <v>0.0128191613675105</v>
       </c>
       <c r="E120" t="n">
-        <v>0.247474996569399</v>
+        <v>0.247474996569398</v>
       </c>
       <c r="F120" t="s">
         <v>1101</v>
@@ -20404,7 +20404,7 @@
         <v>0.0130184057604316</v>
       </c>
       <c r="E121" t="n">
-        <v>0.24920948169969</v>
+        <v>0.249209481699691</v>
       </c>
       <c r="F121" t="s">
         <v>1109</v>
@@ -20607,7 +20607,7 @@
         <v>2.41635984686688</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0135023421528919</v>
+        <v>0.0135023421528918</v>
       </c>
       <c r="E123" t="n">
         <v>0.254201119208989</v>
@@ -24027,7 +24027,7 @@
         <v>35</v>
       </c>
       <c r="T156" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U156" t="n">
         <v>320818.843137255</v>
@@ -24287,7 +24287,7 @@
         <v>2.09123850802625</v>
       </c>
       <c r="D159" t="n">
-        <v>0.019990741169975</v>
+        <v>0.0199907411699751</v>
       </c>
       <c r="E159" t="n">
         <v>0.290056741307027</v>
@@ -25011,7 +25011,7 @@
         <v>1.21762092344371</v>
       </c>
       <c r="D166" t="n">
-        <v>0.0210472208862264</v>
+        <v>0.0210472208862265</v>
       </c>
       <c r="E166" t="n">
         <v>0.292351031578194</v>
@@ -25523,7 +25523,7 @@
         <v>0.867853197341834</v>
       </c>
       <c r="D171" t="n">
-        <v>0.0226620463765856</v>
+        <v>0.0226620463765855</v>
       </c>
       <c r="E171" t="n">
         <v>0.302772694851184</v>
@@ -25729,7 +25729,7 @@
         <v>0.78371578317638</v>
       </c>
       <c r="D173" t="n">
-        <v>0.022815822360676</v>
+        <v>0.0228158223606759</v>
       </c>
       <c r="E173" t="n">
         <v>0.302772694851184</v>
@@ -25983,7 +25983,7 @@
         <v>35</v>
       </c>
       <c r="T175" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U175" t="n">
         <v>14629.5392156863</v>
@@ -26761,7 +26761,7 @@
         <v>1.57761266392044</v>
       </c>
       <c r="D183" t="n">
-        <v>0.02456910025865</v>
+        <v>0.0245691002586501</v>
       </c>
       <c r="E183" t="n">
         <v>0.31093561327336</v>
@@ -26865,10 +26865,10 @@
         <v>0.27905489843125</v>
       </c>
       <c r="D184" t="n">
-        <v>0.024859450574423</v>
+        <v>0.0248594505744229</v>
       </c>
       <c r="E184" t="n">
-        <v>0.312871980157655</v>
+        <v>0.312871980157654</v>
       </c>
       <c r="F184" t="s">
         <v>1610</v>
@@ -27901,7 +27901,7 @@
         <v>1.25376454302494</v>
       </c>
       <c r="D194" t="n">
-        <v>0.0268198605739048</v>
+        <v>0.0268198605739047</v>
       </c>
       <c r="E194" t="n">
         <v>0.320208023246158</v>
@@ -28211,7 +28211,7 @@
         <v>0.934103101296284</v>
       </c>
       <c r="D197" t="n">
-        <v>0.0270112981520271</v>
+        <v>0.027011298152027</v>
       </c>
       <c r="E197" t="n">
         <v>0.320477797866238</v>
@@ -28420,7 +28420,7 @@
         <v>0.0276051011071821</v>
       </c>
       <c r="E199" t="n">
-        <v>0.324146496505984</v>
+        <v>0.324146496505983</v>
       </c>
       <c r="F199" t="s">
         <v>1725</v>
@@ -30573,7 +30573,7 @@
         <v>1.22119471051002</v>
       </c>
       <c r="D220" t="n">
-        <v>0.0313979597922135</v>
+        <v>0.0313979597922136</v>
       </c>
       <c r="E220" t="n">
         <v>0.334574251532132</v>
@@ -30782,7 +30782,7 @@
         <v>0.0318779053495754</v>
       </c>
       <c r="E222" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F222" t="s">
         <v>1908</v>
@@ -30881,10 +30881,10 @@
         <v>2.26264357683325</v>
       </c>
       <c r="D223" t="n">
-        <v>0.0319603715053674</v>
+        <v>0.0319603715053673</v>
       </c>
       <c r="E223" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F223" t="s">
         <v>1918</v>
@@ -30986,7 +30986,7 @@
         <v>0.0320126471951682</v>
       </c>
       <c r="E224" t="n">
-        <v>0.336059033689369</v>
+        <v>0.33605903368937</v>
       </c>
       <c r="F224" t="s">
         <v>1925</v>
@@ -31397,7 +31397,7 @@
         <v>1.78887655907102</v>
       </c>
       <c r="D228" t="n">
-        <v>0.0337919159899818</v>
+        <v>0.0337919159899819</v>
       </c>
       <c r="E228" t="n">
         <v>0.344552495084485</v>
@@ -31415,7 +31415,7 @@
         <v>14.6473805435874</v>
       </c>
       <c r="J228" t="n">
-        <v>3.45545707860451</v>
+        <v>3.4554570786045</v>
       </c>
       <c r="K228" t="s">
         <v>1961</v>
@@ -31499,7 +31499,7 @@
         <v>0.99704828479797</v>
       </c>
       <c r="D229" t="n">
-        <v>0.0338290806249596</v>
+        <v>0.0338290806249597</v>
       </c>
       <c r="E229" t="n">
         <v>0.344552495084485</v>
@@ -32115,7 +32115,7 @@
         <v>0.345489069906911</v>
       </c>
       <c r="D235" t="n">
-        <v>0.0346714061628504</v>
+        <v>0.0346714061628505</v>
       </c>
       <c r="E235" t="n">
         <v>0.344552495084485</v>
@@ -32336,7 +32336,7 @@
         <v>16.7343818564733</v>
       </c>
       <c r="I237" t="n">
-        <v>16.33772736267</v>
+        <v>16.3377273626701</v>
       </c>
       <c r="J237" t="n">
         <v>1.36152590482721</v>
@@ -32425,7 +32425,7 @@
         <v>1.74087635676352</v>
       </c>
       <c r="D238" t="n">
-        <v>0.0350155554167379</v>
+        <v>0.0350155554167378</v>
       </c>
       <c r="E238" t="n">
         <v>0.344552495084485</v>
@@ -33449,7 +33449,7 @@
         <v>1.80708411033922</v>
       </c>
       <c r="D248" t="n">
-        <v>0.037846962738846</v>
+        <v>0.0378469627388461</v>
       </c>
       <c r="E248" t="n">
         <v>0.355763774130317</v>
@@ -34189,7 +34189,7 @@
         <v>27.2048783401882</v>
       </c>
       <c r="J255" t="n">
-        <v>2.160645201853</v>
+        <v>2.16064520185301</v>
       </c>
       <c r="K255" t="s">
         <v>2161</v>
@@ -34375,7 +34375,7 @@
         <v>1.27522696767494</v>
       </c>
       <c r="D257" t="n">
-        <v>0.0394247070068918</v>
+        <v>0.0394247070068917</v>
       </c>
       <c r="E257" t="n">
         <v>0.357433512293212</v>
@@ -35043,7 +35043,7 @@
         <v>35</v>
       </c>
       <c r="T263" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U263" t="n">
         <v>515977.68627451</v>
@@ -35145,7 +35145,7 @@
         <v>35</v>
       </c>
       <c r="T264" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U264" t="n">
         <v>515977.68627451</v>
@@ -35199,7 +35199,7 @@
         <v>0.961685940676187</v>
       </c>
       <c r="D265" t="n">
-        <v>0.0404195812337835</v>
+        <v>0.0404195812337836</v>
       </c>
       <c r="E265" t="n">
         <v>0.357456311668854</v>
@@ -35211,7 +35211,7 @@
         <v>28.0202647722528</v>
       </c>
       <c r="H265" t="n">
-        <v>28.981950712929</v>
+        <v>28.9819507129289</v>
       </c>
       <c r="I265" t="n">
         <v>28.1251759657811</v>
@@ -35410,7 +35410,7 @@
         <v>0.0408089847599079</v>
       </c>
       <c r="E267" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F267" t="s">
         <v>2252</v>
@@ -35512,7 +35512,7 @@
         <v>0.0410740982767807</v>
       </c>
       <c r="E268" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F268" t="s">
         <v>2259</v>
@@ -35614,7 +35614,7 @@
         <v>0.0411672875092047</v>
       </c>
       <c r="E269" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F269" t="s">
         <v>2267</v>
@@ -35718,7 +35718,7 @@
         <v>0.0412637383917675</v>
       </c>
       <c r="E270" t="n">
-        <v>0.358774030749796</v>
+        <v>0.358774030749795</v>
       </c>
       <c r="F270" t="s">
         <v>2276</v>
@@ -37525,7 +37525,7 @@
         <v>42</v>
       </c>
       <c r="T287" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U287" t="n">
         <v>92532.2745098039</v>
@@ -37939,7 +37939,7 @@
         <v>35</v>
       </c>
       <c r="T291" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U291" t="n">
         <v>414179.411764706</v>
@@ -38095,7 +38095,7 @@
         <v>0.954203411581308</v>
       </c>
       <c r="D293" t="n">
-        <v>0.0468029766410783</v>
+        <v>0.0468029766410784</v>
       </c>
       <c r="E293" t="n">
         <v>0.385015325892463</v>
@@ -38705,7 +38705,7 @@
         <v>1.19638760298473</v>
       </c>
       <c r="D299" t="n">
-        <v>0.0483823662658334</v>
+        <v>0.0483823662658333</v>
       </c>
       <c r="E299" t="n">
         <v>0.387625187717942</v>
@@ -39121,7 +39121,7 @@
         <v>1.35134538902765</v>
       </c>
       <c r="D303" t="n">
-        <v>0.0486856279723762</v>
+        <v>0.0486856279723761</v>
       </c>
       <c r="E303" t="n">
         <v>0.387625187717942</v>
@@ -39327,7 +39327,7 @@
         <v>1.43659926223378</v>
       </c>
       <c r="D305" t="n">
-        <v>0.0493091279355317</v>
+        <v>0.0493091279355316</v>
       </c>
       <c r="E305" t="n">
         <v>0.387625187717942</v>
@@ -39887,7 +39887,7 @@
         <v>35</v>
       </c>
       <c r="T310" t="n">
-        <v>80.952380952381</v>
+        <v>80.9523809523809</v>
       </c>
       <c r="U310" t="n">
         <v>177143.539215686</v>

</xml_diff>